<commit_message>
Updated Screenshot Timestamp Format yyyy_MM_dd_HH:mm:ss to yyyy_MM_dd_HH_mm_ss
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t xml:space="preserve">TestCase</t>
   </si>
@@ -43,16 +43,16 @@
     <t xml:space="preserve">v.malkar@smartshiphub.com</t>
   </si>
   <si>
+    <t xml:space="preserve">SUCCESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1v.malkar@smartshiphub.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vaibhav@321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUCCESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">invalid_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1v.malkar@smartshiphub.com</t>
   </si>
   <si>
     <t xml:space="preserve">FAILURE</t>
@@ -362,7 +362,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -398,22 +398,19 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -446,7 +443,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -462,11 +459,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="Vaibhav@321"/>
-    <hyperlink ref="C3" r:id="rId3" display="Vaibhav@321"/>
-    <hyperlink ref="B4" r:id="rId4" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C4" r:id="rId5" display="Vaibhav@3211"/>
-    <hyperlink ref="C5" r:id="rId6" display="Vaibhav@3211"/>
+    <hyperlink ref="C3" r:id="rId2" display="Vaibhav@321"/>
+    <hyperlink ref="B4" r:id="rId3" display="v.malkar@smartshiphub.com"/>
+    <hyperlink ref="C4" r:id="rId4" display="Vaibhav@3211"/>
+    <hyperlink ref="C5" r:id="rId5" display="Vaibhav@3211"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Generate unique Extent report per execution using timestamp
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">TestCase</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">v.malkar@smartshiphub.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Vaibhav@321</t>
+  </si>
+  <si>
     <t xml:space="preserve">SUCCESS</t>
   </si>
   <si>
@@ -50,9 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">1v.malkar@smartshiphub.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaibhav@321</t>
   </si>
   <si>
     <t xml:space="preserve">FAILURE</t>
@@ -362,7 +362,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -398,19 +398,22 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -443,7 +446,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -459,10 +462,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="Vaibhav@321"/>
-    <hyperlink ref="B4" r:id="rId3" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C4" r:id="rId4" display="Vaibhav@3211"/>
-    <hyperlink ref="C5" r:id="rId5" display="Vaibhav@3211"/>
+    <hyperlink ref="C2" r:id="rId2" display="Vaibhav@321"/>
+    <hyperlink ref="C3" r:id="rId3" display="Vaibhav@321"/>
+    <hyperlink ref="B4" r:id="rId4" display="v.malkar@smartshiphub.com"/>
+    <hyperlink ref="C4" r:id="rId5" display="Vaibhav@3211"/>
+    <hyperlink ref="C5" r:id="rId6" display="Vaibhav@3211"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Updated test listener, test data, and cleaned gitignore
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -362,7 +362,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,12 +461,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="Vaibhav@321"/>
-    <hyperlink ref="C3" r:id="rId3" display="Vaibhav@321"/>
-    <hyperlink ref="B4" r:id="rId4" display="v.malkar@smartshiphub.com"/>
-    <hyperlink ref="C4" r:id="rId5" display="Vaibhav@3211"/>
-    <hyperlink ref="C5" r:id="rId6" display="Vaibhav@3211"/>
+    <hyperlink ref="C2" r:id="rId1" display="Vaibhav@321"/>
+    <hyperlink ref="C3" r:id="rId2" display="Vaibhav@321"/>
+    <hyperlink ref="C4" r:id="rId3" display="Vaibhav@3211"/>
+    <hyperlink ref="C5" r:id="rId4" display="Vaibhav@3211"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>